<commit_message>
Standardize spelling and format
</commit_message>
<xml_diff>
--- a/python_worksheets.xlsx
+++ b/python_worksheets.xlsx
@@ -17,12 +17,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="93">
   <si>
     <t>transactions</t>
   </si>
   <si>
-    <t>QTY</t>
+    <t>qty</t>
   </si>
   <si>
     <t>all_sessions</t>
@@ -31,13 +31,13 @@
     <t>user_sessions</t>
   </si>
   <si>
-    <t>ECR</t>
+    <t>ecr</t>
   </si>
   <si>
     <t>month</t>
   </si>
   <si>
-    <t>dim_deviceCategory</t>
+    <t>device_category</t>
   </si>
   <si>
     <t>2012-07</t>
@@ -91,7 +91,10 @@
     <t>relative_dif</t>
   </si>
   <si>
-    <t>addsToCart</t>
+    <t>metric</t>
+  </si>
+  <si>
+    <t>adds_to_cart</t>
   </si>
   <si>
     <t>weekday</t>
@@ -121,7 +124,7 @@
     <t>browser_in_user_sessions</t>
   </si>
   <si>
-    <t>dim_browser</t>
+    <t>browser</t>
   </si>
   <si>
     <t>Safari</t>
@@ -1487,6 +1490,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
@@ -1587,7 +1593,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>107970</v>
@@ -1617,7 +1623,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1637,7 +1643,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>28.91363636363636</v>
@@ -1657,7 +1663,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>28.67738883632923</v>
@@ -1677,7 +1683,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>31.91727272727273</v>
@@ -1697,7 +1703,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>33.47735507246377</v>
@@ -1717,7 +1723,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>33.60964513193812</v>
@@ -1737,7 +1743,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>37.88531711555169</v>
@@ -1757,7 +1763,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>31.10151380231523</v>
@@ -1790,36 +1796,36 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2">
+        <v>140847</v>
+      </c>
+      <c r="C2">
+        <v>263776</v>
+      </c>
+      <c r="D2">
         <v>5952256</v>
-      </c>
-      <c r="C2">
-        <v>140847</v>
-      </c>
-      <c r="D2">
-        <v>263776</v>
       </c>
       <c r="E2">
         <v>0.02366279272934498</v>
@@ -1830,16 +1836,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3">
+        <v>66247</v>
+      </c>
+      <c r="C3">
+        <v>125468</v>
+      </c>
+      <c r="D3">
         <v>2527254</v>
-      </c>
-      <c r="C3">
-        <v>66247</v>
-      </c>
-      <c r="D3">
-        <v>125468</v>
       </c>
       <c r="E3">
         <v>0.02621303596710105</v>
@@ -1850,16 +1856,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4">
+        <v>3046</v>
+      </c>
+      <c r="C4">
+        <v>5113</v>
+      </c>
+      <c r="D4">
         <v>518573</v>
-      </c>
-      <c r="C4">
-        <v>3046</v>
-      </c>
-      <c r="D4">
-        <v>5113</v>
       </c>
       <c r="E4">
         <v>0.005873811401673438</v>
@@ -1870,16 +1876,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5">
+        <v>17376</v>
+      </c>
+      <c r="C5">
+        <v>31279</v>
+      </c>
+      <c r="D5">
         <v>495779</v>
-      </c>
-      <c r="C5">
-        <v>17376</v>
-      </c>
-      <c r="D5">
-        <v>31279</v>
       </c>
       <c r="E5">
         <v>0.03504787415360473</v>
@@ -1890,16 +1896,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6">
+        <v>14373</v>
+      </c>
+      <c r="C6">
+        <v>11016</v>
+      </c>
+      <c r="D6">
         <v>469325</v>
-      </c>
-      <c r="C6">
-        <v>14373</v>
-      </c>
-      <c r="D6">
-        <v>11016</v>
       </c>
       <c r="E6">
         <v>0.0306248335375273</v>
@@ -1910,16 +1916,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B7">
+        <v>6338</v>
+      </c>
+      <c r="C7">
+        <v>11814</v>
+      </c>
+      <c r="D7">
         <v>246329</v>
-      </c>
-      <c r="C7">
-        <v>6338</v>
-      </c>
-      <c r="D7">
-        <v>11814</v>
       </c>
       <c r="E7">
         <v>0.0257298166273561</v>
@@ -1930,16 +1936,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8">
+        <v>289</v>
+      </c>
+      <c r="C8">
+        <v>406</v>
+      </c>
+      <c r="D8">
         <v>98408</v>
-      </c>
-      <c r="C8">
-        <v>289</v>
-      </c>
-      <c r="D8">
-        <v>406</v>
       </c>
       <c r="E8">
         <v>0.002936753109503293</v>
@@ -1950,16 +1956,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9">
+        <v>456</v>
+      </c>
+      <c r="C9">
+        <v>774</v>
+      </c>
+      <c r="D9">
         <v>56632</v>
-      </c>
-      <c r="C9">
-        <v>456</v>
-      </c>
-      <c r="D9">
-        <v>774</v>
       </c>
       <c r="E9">
         <v>0.008051984743607854</v>
@@ -1970,16 +1976,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10">
+        <v>524</v>
+      </c>
+      <c r="C10">
+        <v>836</v>
+      </c>
+      <c r="D10">
         <v>35379</v>
-      </c>
-      <c r="C10">
-        <v>524</v>
-      </c>
-      <c r="D10">
-        <v>836</v>
       </c>
       <c r="E10">
         <v>0.01481104610079426</v>
@@ -1990,16 +1996,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>227</v>
+      </c>
+      <c r="D11">
         <v>5695</v>
-      </c>
-      <c r="C11">
-        <v>100</v>
-      </c>
-      <c r="D11">
-        <v>227</v>
       </c>
       <c r="E11">
         <v>0.01755926251097454</v>
@@ -2010,16 +2016,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
         <v>3865</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
       </c>
       <c r="E12">
         <v>0.001552393272962484</v>
@@ -2030,16 +2036,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
         <v>2359</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -2050,16 +2056,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
         <v>2319</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
-      </c>
-      <c r="D14">
-        <v>8</v>
       </c>
       <c r="E14">
         <v>0.00301854247520483</v>
@@ -2070,16 +2076,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
         <v>1225</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2090,16 +2096,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>86</v>
+      </c>
+      <c r="D16">
         <v>829</v>
-      </c>
-      <c r="C16">
-        <v>29</v>
-      </c>
-      <c r="D16">
-        <v>86</v>
       </c>
       <c r="E16">
         <v>0.03498190591073583</v>
@@ -2110,16 +2116,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
         <v>491</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2130,16 +2136,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
         <v>387</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2150,16 +2156,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19">
-        <v>372</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>372</v>
       </c>
       <c r="E19">
         <v>0.008064516129032258</v>
@@ -2170,16 +2176,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
         <v>272</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
       </c>
       <c r="E20">
         <v>0.007352941176470588</v>
@@ -2190,16 +2196,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
         <v>255</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
       </c>
       <c r="E21">
         <v>0.01176470588235294</v>
@@ -2210,16 +2216,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>6</v>
+      </c>
+      <c r="D22">
         <v>208</v>
-      </c>
-      <c r="C22">
-        <v>5</v>
-      </c>
-      <c r="D22">
-        <v>6</v>
       </c>
       <c r="E22">
         <v>0.02403846153846154</v>
@@ -2230,16 +2236,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
         <v>133</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2250,16 +2256,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
         <v>131</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -2270,16 +2276,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
         <v>117</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2290,16 +2296,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
         <v>101</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -2310,16 +2316,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B27">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>4</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="E27">
         <v>0.05633802816901409</v>
@@ -2330,16 +2336,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
         <v>28</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2350,16 +2356,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
         <v>18</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -2370,16 +2376,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
         <v>17</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -2390,16 +2396,16 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
         <v>17</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -2410,16 +2416,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
         <v>13</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -2430,16 +2436,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
         <v>12</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -2450,16 +2456,16 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
         <v>6</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -2470,16 +2476,16 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
         <v>4</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -2490,16 +2496,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
         <v>4</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -2510,16 +2516,16 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
         <v>4</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -2530,16 +2536,16 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
         <v>3</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -2550,16 +2556,16 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
         <v>2</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -2570,16 +2576,16 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
         <v>2</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -2590,16 +2596,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
         <v>2</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -2610,16 +2616,16 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
         <v>2</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2630,16 +2636,16 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
         <v>2</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -2650,16 +2656,16 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
         <v>2</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -2670,16 +2676,16 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
         <v>2</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -2690,16 +2696,16 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
         <v>2</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -2710,16 +2716,16 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -2730,16 +2736,16 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2750,16 +2756,16 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -2770,16 +2776,16 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2790,16 +2796,16 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51">
         <v>0</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -2810,16 +2816,16 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -2830,7 +2836,7 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -2847,7 +2853,7 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -2864,7 +2870,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -2881,7 +2887,7 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -2898,7 +2904,7 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -2915,7 +2921,7 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B58">
         <v>0</v>

</xml_diff>